<commit_message>
working on data entry membership cards
</commit_message>
<xml_diff>
--- a/public/excel/book1.xlsx
+++ b/public/excel/book1.xlsx
@@ -2092,10 +2092,10 @@
     <t>محمد السيد مصطفى محمد حسين مكرر 1</t>
   </si>
   <si>
-    <t>أشرف وديع رزق مكرر 1</t>
-  </si>
-  <si>
     <t>احمد رشدى معروف مكرر 1</t>
+  </si>
+  <si>
+    <t>أشرف وديع رزق مكرر1</t>
   </si>
 </sst>
 </file>
@@ -2568,8 +2568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C342"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0">
-      <selection activeCell="B254" sqref="B254"/>
+    <sheetView tabSelected="1" topLeftCell="A294" workbookViewId="0">
+      <selection activeCell="C310" sqref="C310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5841,7 +5841,7 @@
         <v>427</v>
       </c>
       <c r="C297" s="6" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
     </row>
     <row r="298" spans="1:3" ht="16.5">
@@ -6336,7 +6336,7 @@
         <v>566</v>
       </c>
       <c r="C342" s="8" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
   </sheetData>

</xml_diff>